<commit_message>
Tried clustering analyses, looked at differences across time
</commit_message>
<xml_diff>
--- a/Arkansas_Data/Data/All_MI_measurements_FILLED_27Jan.xlsx
+++ b/Arkansas_Data/Data/All_MI_measurements_FILLED_27Jan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\Documents\GitHub\Methane_Insight\Arkansas_Data\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101B826C-CFAA-4EA8-9177-33E9FE998ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E9CC88-69D4-4A55-A70D-A8D9FFBD25B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21697" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -536,13 +536,13 @@
   <dimension ref="A1:F558"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E282" sqref="E282"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C200" sqref="C200:E200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>